<commit_message>
added remembering of legend by setting series.
added a legend state value that holds the current legend series names
</commit_message>
<xml_diff>
--- a/components/bower_components/czechrepublicdata.xlsx
+++ b/components/bower_components/czechrepublicdata.xlsx
@@ -53,9 +53,6 @@
     <t>Gross Saving, GDP %</t>
   </si>
   <si>
-    <t>GDP (per capita), Kč</t>
-  </si>
-  <si>
     <t>Population, millions</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>GDP, billions Kč</t>
+  </si>
+  <si>
+    <t>GDP (per capita), K Kč</t>
   </si>
 </sst>
 </file>
@@ -498,29 +498,29 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" customWidth="1"/>
@@ -531,19 +531,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -552,13 +552,13 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -570,16 +570,16 @@
         <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
added normalisation to quiz hints
edited data.
</commit_message>
<xml_diff>
--- a/components/bower_components/czechrepublicdata.xlsx
+++ b/components/bower_components/czechrepublicdata.xlsx
@@ -90,11 +90,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;Kč&quot;;\-#,##0\ &quot;Kč&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;Kč&quot;;\-#,##0.00\ &quot;Kč&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +130,19 @@
       <sz val="8"/>
       <name val="Arial CE"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial CE"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -144,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -176,6 +190,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -197,9 +222,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="% procenta" xfId="2"/>
@@ -495,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -595,8 +629,8 @@
       <c r="B2" s="1">
         <v>1195.8109999999999</v>
       </c>
-      <c r="C2" s="1">
-        <v>2250.7012405999999</v>
+      <c r="C2" s="2">
+        <v>2430.7012405999999</v>
       </c>
       <c r="D2" s="1">
         <v>10.330607000000001</v>
@@ -645,8 +679,8 @@
       <c r="B3" s="1">
         <v>1364.8230000000001</v>
       </c>
-      <c r="C3" s="1">
-        <v>2316.1811048</v>
+      <c r="C3" s="2">
+        <v>2496.1811048</v>
       </c>
       <c r="D3" s="1">
         <v>10.336162</v>
@@ -695,8 +729,8 @@
       <c r="B4" s="1">
         <v>1580.115</v>
       </c>
-      <c r="C4" s="1">
-        <v>2460.2801350999998</v>
+      <c r="C4" s="2">
+        <v>2640.2801350999998</v>
       </c>
       <c r="D4" s="1">
         <v>10.330759</v>
@@ -729,7 +763,9 @@
       <c r="P4" s="1">
         <v>7.23</v>
       </c>
-      <c r="Q4" s="1"/>
+      <c r="Q4" s="1">
+        <v>11</v>
+      </c>
       <c r="R4" s="1">
         <v>0.45756163317226911</v>
       </c>
@@ -747,8 +783,8 @@
       <c r="B5" s="1">
         <v>1812.6220000000001</v>
       </c>
-      <c r="C5" s="1">
-        <v>2565.6489892</v>
+      <c r="C5" s="2">
+        <v>2759.6210000000001</v>
       </c>
       <c r="D5" s="1">
         <v>10.315353</v>
@@ -781,7 +817,9 @@
       <c r="P5" s="1">
         <v>-1.5620000000000001</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="10">
+        <v>11.3</v>
+      </c>
       <c r="R5" s="1">
         <v>-8.6173509976156082E-2</v>
       </c>
@@ -799,8 +837,8 @@
       <c r="B6" s="1">
         <v>1953.3109999999999</v>
       </c>
-      <c r="C6" s="1">
-        <v>2548.3495557000001</v>
+      <c r="C6" s="2">
+        <v>2740.2440000000001</v>
       </c>
       <c r="D6" s="1">
         <v>10.303642</v>
@@ -833,7 +871,9 @@
       <c r="P6" s="1">
         <v>-15.717000000000001</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="1">
+        <v>12.5</v>
+      </c>
       <c r="R6" s="1">
         <v>-0.80463377311651862</v>
       </c>
@@ -851,8 +891,8 @@
       <c r="B7" s="1">
         <v>2142.587</v>
       </c>
-      <c r="C7" s="1">
-        <v>2540.2959386000002</v>
+      <c r="C7" s="2">
+        <v>2731.971</v>
       </c>
       <c r="D7" s="1">
         <v>10.294943</v>
@@ -885,7 +925,9 @@
       <c r="P7" s="1">
         <v>-29.331</v>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="1">
+        <v>14.9</v>
+      </c>
       <c r="R7" s="1">
         <v>-1.3689525792884956</v>
       </c>
@@ -896,15 +938,15 @@
         <v>9.0860254449410931</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" ht="15.75" customHeight="1">
       <c r="A8" s="1">
         <v>1999</v>
       </c>
       <c r="B8" s="1">
         <v>2237.3000000000002</v>
       </c>
-      <c r="C8" s="1">
-        <v>2576.8266699999999</v>
+      <c r="C8" s="2">
+        <v>2766.7359999999999</v>
       </c>
       <c r="D8" s="1">
         <v>10.282783999999999</v>
@@ -937,7 +979,9 @@
       <c r="P8" s="1">
         <v>-29.634</v>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1">
+        <v>9.6</v>
+      </c>
       <c r="R8" s="1">
         <v>-1.324542975908461</v>
       </c>
@@ -955,8 +999,8 @@
       <c r="B9" s="1">
         <v>2372.63</v>
       </c>
-      <c r="C9" s="1">
-        <v>2687.4791132999999</v>
+      <c r="C9" s="2">
+        <v>2895.2339999999999</v>
       </c>
       <c r="D9" s="1">
         <v>10.272503</v>
@@ -990,7 +1034,7 @@
         <v>-46.061</v>
       </c>
       <c r="Q9" s="1">
-        <v>7.38</v>
+        <v>5.43</v>
       </c>
       <c r="R9" s="1">
         <v>-1.9413477870548714</v>
@@ -1009,8 +1053,8 @@
       <c r="B10" s="1">
         <v>2562.6790000000001</v>
       </c>
-      <c r="C10" s="1">
-        <v>2769.4881104000001</v>
+      <c r="C10" s="2">
+        <v>2983.2489999999998</v>
       </c>
       <c r="D10" s="1">
         <v>10.224192</v>
@@ -1067,8 +1111,8 @@
       <c r="B11" s="1">
         <v>2674.634</v>
       </c>
-      <c r="C11" s="1">
-        <v>2815.1001848999999</v>
+      <c r="C11" s="2">
+        <v>3029.8110000000001</v>
       </c>
       <c r="D11" s="1">
         <v>10.200773999999999</v>
@@ -1111,7 +1155,7 @@
         <v>-45.716000000000001</v>
       </c>
       <c r="Q11" s="1">
-        <v>4.1500000000000004</v>
+        <v>4.75</v>
       </c>
       <c r="R11" s="1">
         <v>-1.7092432086034948</v>
@@ -1130,8 +1174,8 @@
       <c r="B12" s="1">
         <v>2801.163</v>
       </c>
-      <c r="C12" s="1">
-        <v>2916.4956609999999</v>
+      <c r="C12" s="2">
+        <v>3138.8580000000002</v>
       </c>
       <c r="D12" s="1">
         <v>10.201651</v>
@@ -1174,7 +1218,7 @@
         <v>-109.053</v>
       </c>
       <c r="Q12" s="1">
-        <v>4.82</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="R12" s="1">
         <v>-3.8931329594172137</v>
@@ -1193,8 +1237,8 @@
       <c r="B13" s="1">
         <v>3057.66</v>
       </c>
-      <c r="C13" s="1">
-        <v>3060.7880080999998</v>
+      <c r="C13" s="2">
+        <v>3289.2240000000002</v>
       </c>
       <c r="D13" s="1">
         <v>10.206923</v>
@@ -1237,7 +1281,7 @@
         <v>-93.683999999999997</v>
       </c>
       <c r="Q13" s="1">
-        <v>4.1399999999999997</v>
+        <v>2</v>
       </c>
       <c r="R13" s="1">
         <v>-3.0639116186888011</v>
@@ -1256,8 +1300,8 @@
       <c r="B14" s="1">
         <v>3257.9720000000002</v>
       </c>
-      <c r="C14" s="1">
-        <v>3257.9720000000002</v>
+      <c r="C14" s="2">
+        <v>3503.4989999999998</v>
       </c>
       <c r="D14" s="1">
         <v>10.234092</v>
@@ -1300,7 +1344,7 @@
         <v>-56.338000000000001</v>
       </c>
       <c r="Q14" s="1">
-        <v>3.61</v>
+        <v>2.5</v>
       </c>
       <c r="R14" s="1">
         <v>-1.7292352420462791</v>
@@ -1319,8 +1363,8 @@
       <c r="B15" s="1">
         <v>3507.1309999999999</v>
       </c>
-      <c r="C15" s="1">
-        <v>3482.0078868999999</v>
+      <c r="C15" s="2">
+        <v>3751.2109999999998</v>
       </c>
       <c r="D15" s="1">
         <v>10.266646</v>
@@ -1363,7 +1407,7 @@
         <v>-97.58</v>
       </c>
       <c r="Q15" s="1">
-        <v>3.77</v>
+        <v>2</v>
       </c>
       <c r="R15" s="1">
         <v>-2.7823311989201427</v>
@@ -1382,8 +1426,8 @@
       <c r="B16" s="1">
         <v>3831.819</v>
       </c>
-      <c r="C16" s="1">
-        <v>3674.5373768999998</v>
+      <c r="C16" s="2">
+        <v>3958.0729999999999</v>
       </c>
       <c r="D16" s="1">
         <v>10.322689</v>
@@ -1426,7 +1470,7 @@
         <v>-66.391999999999996</v>
       </c>
       <c r="Q16" s="1">
-        <v>4.68</v>
+        <v>2.5</v>
       </c>
       <c r="R16" s="1">
         <v>-1.7326496893511931</v>
@@ -1445,8 +1489,8 @@
       <c r="B17" s="1">
         <v>4015.346</v>
       </c>
-      <c r="C17" s="1">
-        <v>3774.1524525999998</v>
+      <c r="C17" s="2">
+        <v>4058.5740000000001</v>
       </c>
       <c r="D17" s="1">
         <v>10.429691999999999</v>
@@ -1489,7 +1533,7 @@
         <v>-20.003</v>
       </c>
       <c r="Q17" s="1">
-        <v>4.3</v>
+        <v>3.5</v>
       </c>
       <c r="R17" s="1">
         <v>-0.49816379460200938</v>
@@ -1508,8 +1552,8 @@
       <c r="B18" s="1">
         <v>3921.8270000000002</v>
       </c>
-      <c r="C18" s="1">
-        <v>3591.4160941</v>
+      <c r="C18" s="2">
+        <v>3867.8029999999999</v>
       </c>
       <c r="D18" s="1">
         <v>10.491491999999999</v>
@@ -1552,7 +1596,7 @@
         <v>-192.39400000000001</v>
       </c>
       <c r="Q18" s="1">
-        <v>3.98</v>
+        <v>2.25</v>
       </c>
       <c r="R18" s="1">
         <v>-4.9057237863883341</v>
@@ -1571,8 +1615,8 @@
       <c r="B19" s="1">
         <v>3953.6509999999998</v>
       </c>
-      <c r="C19" s="1">
-        <v>3673.8423145000002</v>
+      <c r="C19" s="2">
+        <v>3950.607</v>
       </c>
       <c r="D19" s="1">
         <v>10.517246999999999</v>
@@ -1615,7 +1659,7 @@
         <v>-156.416</v>
       </c>
       <c r="Q19" s="1">
-        <v>3.89</v>
+        <v>1</v>
       </c>
       <c r="R19" s="1">
         <v>-3.956241964705534</v>
@@ -1634,8 +1678,8 @@
       <c r="B20" s="1">
         <v>4022.41</v>
       </c>
-      <c r="C20" s="1">
-        <v>3745.988488</v>
+      <c r="C20" s="2">
+        <v>4028.489</v>
       </c>
       <c r="D20" s="1">
         <v>10.496672</v>
@@ -1678,7 +1722,7 @@
         <v>-142.77099999999999</v>
       </c>
       <c r="Q20" s="1">
-        <v>3.7</v>
+        <v>0.76</v>
       </c>
       <c r="R20" s="1">
         <v>-3.5493853570371989</v>
@@ -1697,8 +1741,8 @@
       <c r="B21" s="1">
         <v>4047.6750000000002</v>
       </c>
-      <c r="C21" s="1">
-        <v>3715.7058840999998</v>
+      <c r="C21" s="2">
+        <v>3999.0720000000001</v>
       </c>
       <c r="D21" s="1">
         <v>10.509285999999999</v>
@@ -1741,7 +1785,7 @@
         <v>-101</v>
       </c>
       <c r="Q21" s="1">
-        <v>1.92</v>
+        <v>0.76</v>
       </c>
       <c r="R21" s="1">
         <v>-2.4952596243522516</v>
@@ -1760,8 +1804,8 @@
       <c r="B22" s="1">
         <v>4086.26</v>
       </c>
-      <c r="C22" s="1">
-        <v>3689.6345405000002</v>
+      <c r="C22" s="2">
+        <v>3970.7130000000002</v>
       </c>
       <c r="D22" s="1">
         <v>10.510719</v>
@@ -1804,7 +1848,7 @@
         <v>-81.263999999999996</v>
       </c>
       <c r="Q22" s="1">
-        <v>2.2000000000000002</v>
+        <v>0.04</v>
       </c>
       <c r="R22" s="1">
         <v>-1.9887238452766096</v>
@@ -1823,7 +1867,9 @@
       <c r="B23" s="1">
         <v>4298.2</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="3">
+        <v>4056.26</v>
+      </c>
       <c r="D23" s="1">
         <v>10.7</v>
       </c>
@@ -1851,9 +1897,11 @@
         <v>-77.781999999999996</v>
       </c>
       <c r="Q23" s="1">
-        <v>0.67</v>
-      </c>
-      <c r="R23" s="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="R23" s="1">
+        <v>-2.1</v>
+      </c>
       <c r="S23" s="1">
         <v>1663.7</v>
       </c>
@@ -1862,6 +1910,106 @@
         <v>38.706900563026387</v>
       </c>
     </row>
+    <row r="24" spans="1:20" s="4" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="25" spans="1:20" s="4" customFormat="1"/>
+    <row r="26" spans="1:20" s="4" customFormat="1">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" s="4" customFormat="1">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:20" s="4" customFormat="1">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:20" s="4" customFormat="1">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:20" s="4" customFormat="1">
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:20" s="4" customFormat="1">
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:20" s="4" customFormat="1">
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="3:4" s="4" customFormat="1">
+      <c r="C33" s="7"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="3:4" s="4" customFormat="1">
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="3:4" s="4" customFormat="1">
+      <c r="C35" s="7"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="3:4" s="4" customFormat="1">
+      <c r="C36" s="7"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="3:4" s="4" customFormat="1">
+      <c r="C37" s="7"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="3:4" s="4" customFormat="1">
+      <c r="C38" s="7"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="3:4" s="4" customFormat="1">
+      <c r="C39" s="7"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="3:4" s="4" customFormat="1">
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="3:4" s="4" customFormat="1">
+      <c r="C41" s="7"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="3:4" s="4" customFormat="1">
+      <c r="C42" s="7"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="3:4" s="4" customFormat="1">
+      <c r="C43" s="7"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="3:4" s="4" customFormat="1">
+      <c r="C44" s="7"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="3:4" s="4" customFormat="1">
+      <c r="C45" s="7"/>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="3:4" s="4" customFormat="1">
+      <c r="C46" s="7"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="3:4" s="4" customFormat="1">
+      <c r="C47" s="7"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="3:4" s="4" customFormat="1">
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" s="4" customFormat="1"/>
+    <row r="50" s="4" customFormat="1"/>
+    <row r="51" s="4" customFormat="1"/>
+    <row r="52" s="4" customFormat="1"/>
+    <row r="53" s="4" customFormat="1"/>
+    <row r="54" s="4" customFormat="1"/>
+    <row r="55" s="4" customFormat="1"/>
+    <row r="56" s="4" customFormat="1"/>
+    <row r="57" s="4" customFormat="1"/>
+    <row r="58" s="4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>